<commit_message>
changed initial data, WRITE ALL UNITE TEST BEFORE CODE SMTHNG ELSE
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/test.xlsx
+++ b/src/main/resources/xlsx/test.xlsx
@@ -17,6 +17,21 @@
     <t>Monday</t>
   </si>
   <si>
+    <t>Math1-1</t>
+  </si>
+  <si>
+    <t>Math1-2</t>
+  </si>
+  <si>
+    <t>Phys1-3</t>
+  </si>
+  <si>
+    <t>Litr1-4</t>
+  </si>
+  <si>
+    <t>Math1-5</t>
+  </si>
+  <si>
     <t>Russian1-1</t>
   </si>
   <si>
@@ -26,70 +41,55 @@
     <t>English1-3</t>
   </si>
   <si>
-    <t>Litr1-4</t>
+    <t>English1-4</t>
+  </si>
+  <si>
+    <t>Litr1-5</t>
+  </si>
+  <si>
+    <t>Phys1-1</t>
+  </si>
+  <si>
+    <t>Litr1-2</t>
+  </si>
+  <si>
+    <t>Litr1-3</t>
+  </si>
+  <si>
+    <t>Math1-4</t>
   </si>
   <si>
     <t>Russian1-5</t>
   </si>
   <si>
-    <t>Math1-1</t>
-  </si>
-  <si>
-    <t>Math1-2</t>
-  </si>
-  <si>
-    <t>Phys1-3</t>
-  </si>
-  <si>
-    <t>Math1-4</t>
-  </si>
-  <si>
-    <t>Litr1-5</t>
-  </si>
-  <si>
-    <t>Phys1-1</t>
-  </si>
-  <si>
-    <t>Litr1-2</t>
-  </si>
-  <si>
-    <t>Litr1-3</t>
-  </si>
-  <si>
-    <t>English1-4</t>
-  </si>
-  <si>
-    <t>Math1-5</t>
-  </si>
-  <si>
     <t>Tuesday</t>
   </si>
   <si>
+    <t>English2-1</t>
+  </si>
+  <si>
+    <t>Math2-2</t>
+  </si>
+  <si>
+    <t>Math2-3</t>
+  </si>
+  <si>
+    <t>English2-4</t>
+  </si>
+  <si>
+    <t>Phys2-5</t>
+  </si>
+  <si>
     <t>Math2-1</t>
   </si>
   <si>
-    <t>Phys2-2</t>
+    <t>English2-2</t>
   </si>
   <si>
     <t>Phys2-3</t>
   </si>
   <si>
-    <t>Math2-4</t>
-  </si>
-  <si>
-    <t>Phys2-5</t>
-  </si>
-  <si>
-    <t>English2-1</t>
-  </si>
-  <si>
-    <t>Math2-2</t>
-  </si>
-  <si>
-    <t>Math2-3</t>
-  </si>
-  <si>
-    <t>English2-4</t>
+    <t>Phys2-4</t>
   </si>
   <si>
     <t>Math2-5</t>
@@ -98,61 +98,61 @@
     <t>Wednesday</t>
   </si>
   <si>
+    <t>English3-1</t>
+  </si>
+  <si>
+    <t>Russian3-2</t>
+  </si>
+  <si>
+    <t>English3-3</t>
+  </si>
+  <si>
+    <t>Phys3-4</t>
+  </si>
+  <si>
+    <t>English3-5</t>
+  </si>
+  <si>
     <t>Phys3-1</t>
   </si>
   <si>
     <t>Phys3-2</t>
   </si>
   <si>
-    <t>English3-3</t>
+    <t>Phys3-3</t>
   </si>
   <si>
     <t>Litra3-4</t>
   </si>
   <si>
-    <t>English3-5</t>
+    <t>Phys3-5</t>
   </si>
   <si>
     <t>Russian3-1</t>
   </si>
   <si>
-    <t>Russian3-2</t>
-  </si>
-  <si>
-    <t>Russian3-3</t>
-  </si>
-  <si>
-    <t>Phys3-4</t>
-  </si>
-  <si>
-    <t>Phys3-5</t>
-  </si>
-  <si>
-    <t>English3-1</t>
-  </si>
-  <si>
     <t>Thursday</t>
   </si>
   <si>
+    <t>Math4-1</t>
+  </si>
+  <si>
+    <t>Phys4-2</t>
+  </si>
+  <si>
+    <t>Phys4-3</t>
+  </si>
+  <si>
+    <t>Math4-4</t>
+  </si>
+  <si>
+    <t>Math4-5</t>
+  </si>
+  <si>
     <t>English4-1</t>
   </si>
   <si>
-    <t>Phys4-2</t>
-  </si>
-  <si>
-    <t>Phys4-3</t>
-  </si>
-  <si>
-    <t>Math4-4</t>
-  </si>
-  <si>
-    <t>Math4-5</t>
-  </si>
-  <si>
-    <t>Math4-1</t>
-  </si>
-  <si>
-    <t>Math4-2</t>
+    <t>English4-2</t>
   </si>
   <si>
     <t>Math4-3</t>
@@ -170,13 +170,13 @@
     <t>Russian5-1</t>
   </si>
   <si>
-    <t>Phys5-2</t>
+    <t>Russian5-2</t>
   </si>
   <si>
     <t>Phys5-3</t>
   </si>
   <si>
-    <t>Phys5-4</t>
+    <t>Russian5-4</t>
   </si>
   <si>
     <t>Phys5-5</t>

</xml_diff>

<commit_message>
prepare to break xlsparser::parse()
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/test.xlsx
+++ b/src/main/resources/xlsx/test.xlsx
@@ -17,61 +17,76 @@
     <t>Monday</t>
   </si>
   <si>
+    <t>Math1-1</t>
+  </si>
+  <si>
+    <t>Math1-2</t>
+  </si>
+  <si>
+    <t>Litr1-3</t>
+  </si>
+  <si>
+    <t>Math1-4</t>
+  </si>
+  <si>
+    <t>Russian1-5</t>
+  </si>
+  <si>
     <t>Phys1-1</t>
   </si>
   <si>
-    <t>Math1-2</t>
+    <t>Russian1-2</t>
+  </si>
+  <si>
+    <t>Phys1-3</t>
+  </si>
+  <si>
+    <t>English1-4</t>
+  </si>
+  <si>
+    <t>Math1-5</t>
+  </si>
+  <si>
+    <t>Russian1-1</t>
+  </si>
+  <si>
+    <t>Litr1-2</t>
   </si>
   <si>
     <t>English1-3</t>
   </si>
   <si>
-    <t>English1-4</t>
-  </si>
-  <si>
-    <t>Russian1-5</t>
-  </si>
-  <si>
-    <t>Math1-1</t>
-  </si>
-  <si>
-    <t>Russian1-2</t>
-  </si>
-  <si>
-    <t>Phys1-3</t>
-  </si>
-  <si>
     <t>Litr1-4</t>
   </si>
   <si>
-    <t>Math1-5</t>
-  </si>
-  <si>
-    <t>Russian1-1</t>
-  </si>
-  <si>
-    <t>Litr1-2</t>
-  </si>
-  <si>
-    <t>Litr1-3</t>
-  </si>
-  <si>
-    <t>Math1-4</t>
-  </si>
-  <si>
     <t>Litr1-5</t>
   </si>
   <si>
     <t>Tuesday</t>
   </si>
   <si>
+    <t>Math2-1</t>
+  </si>
+  <si>
+    <t>Phys2-2</t>
+  </si>
+  <si>
+    <t>Phys2-3</t>
+  </si>
+  <si>
+    <t>Math2-4</t>
+  </si>
+  <si>
+    <t>Phys2-5</t>
+  </si>
+  <si>
     <t>English2-1</t>
   </si>
   <si>
-    <t>English2-2</t>
-  </si>
-  <si>
-    <t>Phys2-3</t>
+    <t>Math2-2</t>
+  </si>
+  <si>
+    <t>Math2-3</t>
   </si>
   <si>
     <t>English2-4</t>
@@ -80,87 +95,72 @@
     <t>Math2-5</t>
   </si>
   <si>
-    <t>Math2-1</t>
-  </si>
-  <si>
-    <t>Phys2-2</t>
-  </si>
-  <si>
-    <t>Math2-3</t>
-  </si>
-  <si>
-    <t>Math2-4</t>
-  </si>
-  <si>
-    <t>Phys2-5</t>
-  </si>
-  <si>
     <t>Wednesday</t>
   </si>
   <si>
+    <t>Russian3-1</t>
+  </si>
+  <si>
+    <t>Phys3-2</t>
+  </si>
+  <si>
+    <t>Russian3-3</t>
+  </si>
+  <si>
+    <t>Phys3-4</t>
+  </si>
+  <si>
+    <t>Litra3-5</t>
+  </si>
+  <si>
+    <t>Phys3-1</t>
+  </si>
+  <si>
+    <t>Russian3-2</t>
+  </si>
+  <si>
+    <t>Phys3-3</t>
+  </si>
+  <si>
+    <t>Litra3-4</t>
+  </si>
+  <si>
+    <t>Phys3-5</t>
+  </si>
+  <si>
     <t>English3-1</t>
   </si>
   <si>
-    <t>Russian3-2</t>
-  </si>
-  <si>
-    <t>English3-3</t>
-  </si>
-  <si>
-    <t>Litra3-4</t>
-  </si>
-  <si>
-    <t>Phys3-5</t>
-  </si>
-  <si>
-    <t>Phys3-1</t>
-  </si>
-  <si>
-    <t>Phys3-2</t>
-  </si>
-  <si>
-    <t>Phys3-3</t>
-  </si>
-  <si>
-    <t>Phys3-4</t>
-  </si>
-  <si>
-    <t>English3-5</t>
-  </si>
-  <si>
-    <t>Russian3-1</t>
-  </si>
-  <si>
     <t>Thursday</t>
   </si>
   <si>
+    <t>English4-1</t>
+  </si>
+  <si>
+    <t>Phys4-2</t>
+  </si>
+  <si>
+    <t>Phys4-3</t>
+  </si>
+  <si>
+    <t>Math4-4</t>
+  </si>
+  <si>
+    <t>Math4-5</t>
+  </si>
+  <si>
     <t>Math4-1</t>
   </si>
   <si>
-    <t>Phys4-2</t>
-  </si>
-  <si>
-    <t>Phys4-3</t>
+    <t>Math4-2</t>
+  </si>
+  <si>
+    <t>Math4-3</t>
   </si>
   <si>
     <t>Phys4-4</t>
   </si>
   <si>
-    <t>Math4-5</t>
-  </si>
-  <si>
-    <t>English4-1</t>
-  </si>
-  <si>
-    <t>English4-2</t>
-  </si>
-  <si>
-    <t>Math4-3</t>
-  </si>
-  <si>
-    <t>Math4-4</t>
-  </si>
-  <si>
     <t>English4-5</t>
   </si>
   <si>
@@ -170,7 +170,7 @@
     <t>Russian5-1</t>
   </si>
   <si>
-    <t>Phys5-2</t>
+    <t>Russian5-2</t>
   </si>
   <si>
     <t>Phys5-3</t>

</xml_diff>

<commit_message>
seems like its all good
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/test.xlsx
+++ b/src/main/resources/xlsx/test.xlsx
@@ -17,78 +17,78 @@
     <t>Monday</t>
   </si>
   <si>
+    <t>Phys1-1</t>
+  </si>
+  <si>
+    <t>Russian1-2</t>
+  </si>
+  <si>
+    <t>Litr1-3</t>
+  </si>
+  <si>
+    <t>English1-4</t>
+  </si>
+  <si>
+    <t>Math1-5</t>
+  </si>
+  <si>
+    <t>Russian1-1</t>
+  </si>
+  <si>
+    <t>Math1-2</t>
+  </si>
+  <si>
+    <t>Phys1-3</t>
+  </si>
+  <si>
+    <t>Math1-4</t>
+  </si>
+  <si>
+    <t>Litr1-5</t>
+  </si>
+  <si>
     <t>Math1-1</t>
   </si>
   <si>
-    <t>Math1-2</t>
-  </si>
-  <si>
-    <t>Litr1-3</t>
-  </si>
-  <si>
-    <t>Math1-4</t>
+    <t>Litr1-2</t>
+  </si>
+  <si>
+    <t>English1-3</t>
+  </si>
+  <si>
+    <t>Litr1-4</t>
   </si>
   <si>
     <t>Russian1-5</t>
   </si>
   <si>
-    <t>Phys1-1</t>
-  </si>
-  <si>
-    <t>Russian1-2</t>
-  </si>
-  <si>
-    <t>Phys1-3</t>
-  </si>
-  <si>
-    <t>English1-4</t>
-  </si>
-  <si>
-    <t>Math1-5</t>
-  </si>
-  <si>
-    <t>Russian1-1</t>
-  </si>
-  <si>
-    <t>Litr1-2</t>
-  </si>
-  <si>
-    <t>English1-3</t>
-  </si>
-  <si>
-    <t>Litr1-4</t>
-  </si>
-  <si>
-    <t>Litr1-5</t>
-  </si>
-  <si>
     <t>Tuesday</t>
   </si>
   <si>
     <t>Math2-1</t>
   </si>
   <si>
+    <t>Math2-2</t>
+  </si>
+  <si>
+    <t>Math2-3</t>
+  </si>
+  <si>
+    <t>Phys2-4</t>
+  </si>
+  <si>
+    <t>Phys2-5</t>
+  </si>
+  <si>
+    <t>English2-1</t>
+  </si>
+  <si>
     <t>Phys2-2</t>
   </si>
   <si>
     <t>Phys2-3</t>
   </si>
   <si>
-    <t>Math2-4</t>
-  </si>
-  <si>
-    <t>Phys2-5</t>
-  </si>
-  <si>
-    <t>English2-1</t>
-  </si>
-  <si>
-    <t>Math2-2</t>
-  </si>
-  <si>
-    <t>Math2-3</t>
-  </si>
-  <si>
     <t>English2-4</t>
   </si>
   <si>
@@ -101,43 +101,58 @@
     <t>Russian3-1</t>
   </si>
   <si>
+    <t>Russian3-2</t>
+  </si>
+  <si>
+    <t>Phys3-3</t>
+  </si>
+  <si>
+    <t>Phys3-4</t>
+  </si>
+  <si>
+    <t>Litra3-5</t>
+  </si>
+  <si>
+    <t>English3-1</t>
+  </si>
+  <si>
     <t>Phys3-2</t>
   </si>
   <si>
     <t>Russian3-3</t>
   </si>
   <si>
-    <t>Phys3-4</t>
-  </si>
-  <si>
-    <t>Litra3-5</t>
+    <t>Litra3-4</t>
+  </si>
+  <si>
+    <t>English3-5</t>
   </si>
   <si>
     <t>Phys3-1</t>
   </si>
   <si>
-    <t>Russian3-2</t>
-  </si>
-  <si>
-    <t>Phys3-3</t>
-  </si>
-  <si>
-    <t>Litra3-4</t>
-  </si>
-  <si>
-    <t>Phys3-5</t>
-  </si>
-  <si>
-    <t>English3-1</t>
-  </si>
-  <si>
     <t>Thursday</t>
   </si>
   <si>
     <t>English4-1</t>
   </si>
   <si>
-    <t>Phys4-2</t>
+    <t>English4-2</t>
+  </si>
+  <si>
+    <t>Math4-3</t>
+  </si>
+  <si>
+    <t>Phys4-4</t>
+  </si>
+  <si>
+    <t>Math4-5</t>
+  </si>
+  <si>
+    <t>Math4-1</t>
+  </si>
+  <si>
+    <t>Math4-2</t>
   </si>
   <si>
     <t>Phys4-3</t>
@@ -146,21 +161,6 @@
     <t>Math4-4</t>
   </si>
   <si>
-    <t>Math4-5</t>
-  </si>
-  <si>
-    <t>Math4-1</t>
-  </si>
-  <si>
-    <t>Math4-2</t>
-  </si>
-  <si>
-    <t>Math4-3</t>
-  </si>
-  <si>
-    <t>Phys4-4</t>
-  </si>
-  <si>
     <t>English4-5</t>
   </si>
   <si>
@@ -170,16 +170,16 @@
     <t>Russian5-1</t>
   </si>
   <si>
-    <t>Russian5-2</t>
+    <t>Phys5-2</t>
   </si>
   <si>
     <t>Phys5-3</t>
   </si>
   <si>
-    <t>Phys5-4</t>
-  </si>
-  <si>
-    <t>Math5-5</t>
+    <t>Math5-4</t>
+  </si>
+  <si>
+    <t>Phys5-5</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
trying to refactor PropertiesExtractor
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/test.xlsx
+++ b/src/main/resources/xlsx/test.xlsx
@@ -20,54 +20,69 @@
     <t>Phys1-1</t>
   </si>
   <si>
+    <t>Litr1-2</t>
+  </si>
+  <si>
+    <t>Phys1-3</t>
+  </si>
+  <si>
+    <t>English1-4</t>
+  </si>
+  <si>
+    <t>Russian1-5</t>
+  </si>
+  <si>
+    <t>Russian1-1</t>
+  </si>
+  <si>
     <t>Russian1-2</t>
   </si>
   <si>
     <t>Litr1-3</t>
   </si>
   <si>
-    <t>English1-4</t>
+    <t>Litr1-4</t>
+  </si>
+  <si>
+    <t>Litr1-5</t>
+  </si>
+  <si>
+    <t>Math1-1</t>
+  </si>
+  <si>
+    <t>Math1-2</t>
+  </si>
+  <si>
+    <t>English1-3</t>
+  </si>
+  <si>
+    <t>Math1-4</t>
   </si>
   <si>
     <t>Math1-5</t>
   </si>
   <si>
-    <t>Russian1-1</t>
-  </si>
-  <si>
-    <t>Math1-2</t>
-  </si>
-  <si>
-    <t>Phys1-3</t>
-  </si>
-  <si>
-    <t>Math1-4</t>
-  </si>
-  <si>
-    <t>Litr1-5</t>
-  </si>
-  <si>
-    <t>Math1-1</t>
-  </si>
-  <si>
-    <t>Litr1-2</t>
-  </si>
-  <si>
-    <t>English1-3</t>
-  </si>
-  <si>
-    <t>Litr1-4</t>
-  </si>
-  <si>
-    <t>Russian1-5</t>
-  </si>
-  <si>
     <t>Tuesday</t>
   </si>
   <si>
     <t>Math2-1</t>
   </si>
   <si>
+    <t>Phys2-2</t>
+  </si>
+  <si>
+    <t>Phys2-3</t>
+  </si>
+  <si>
+    <t>English2-4</t>
+  </si>
+  <si>
+    <t>Math2-5</t>
+  </si>
+  <si>
+    <t>English2-1</t>
+  </si>
+  <si>
     <t>Math2-2</t>
   </si>
   <si>
@@ -80,24 +95,24 @@
     <t>Phys2-5</t>
   </si>
   <si>
-    <t>English2-1</t>
-  </si>
-  <si>
-    <t>Phys2-2</t>
-  </si>
-  <si>
-    <t>Phys2-3</t>
-  </si>
-  <si>
-    <t>English2-4</t>
-  </si>
-  <si>
-    <t>Math2-5</t>
-  </si>
-  <si>
     <t>Wednesday</t>
   </si>
   <si>
+    <t>English3-1</t>
+  </si>
+  <si>
+    <t>Phys3-2</t>
+  </si>
+  <si>
+    <t>Russian3-3</t>
+  </si>
+  <si>
+    <t>Litra3-4</t>
+  </si>
+  <si>
+    <t>English3-5</t>
+  </si>
+  <si>
     <t>Russian3-1</t>
   </si>
   <si>
@@ -113,21 +128,6 @@
     <t>Litra3-5</t>
   </si>
   <si>
-    <t>English3-1</t>
-  </si>
-  <si>
-    <t>Phys3-2</t>
-  </si>
-  <si>
-    <t>Russian3-3</t>
-  </si>
-  <si>
-    <t>Litra3-4</t>
-  </si>
-  <si>
-    <t>English3-5</t>
-  </si>
-  <si>
     <t>Phys3-1</t>
   </si>
   <si>
@@ -140,24 +140,24 @@
     <t>English4-2</t>
   </si>
   <si>
+    <t>Phys4-3</t>
+  </si>
+  <si>
+    <t>Phys4-4</t>
+  </si>
+  <si>
+    <t>Math4-5</t>
+  </si>
+  <si>
+    <t>Math4-1</t>
+  </si>
+  <si>
+    <t>Math4-2</t>
+  </si>
+  <si>
     <t>Math4-3</t>
   </si>
   <si>
-    <t>Phys4-4</t>
-  </si>
-  <si>
-    <t>Math4-5</t>
-  </si>
-  <si>
-    <t>Math4-1</t>
-  </si>
-  <si>
-    <t>Math4-2</t>
-  </si>
-  <si>
-    <t>Phys4-3</t>
-  </si>
-  <si>
     <t>Math4-4</t>
   </si>
   <si>
@@ -176,7 +176,7 @@
     <t>Phys5-3</t>
   </si>
   <si>
-    <t>Math5-4</t>
+    <t>Phys5-4</t>
   </si>
   <si>
     <t>Phys5-5</t>

</xml_diff>

<commit_message>
some for changed to streams
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/test.xlsx
+++ b/src/main/resources/xlsx/test.xlsx
@@ -14,57 +14,57 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
+    <t>Math1-1</t>
+  </si>
+  <si>
+    <t>Math1-2</t>
+  </si>
+  <si>
+    <t>Phys1-3</t>
+  </si>
+  <si>
+    <t>Litr1-4</t>
+  </si>
+  <si>
+    <t>Litr1-5</t>
+  </si>
+  <si>
     <t>Phys1-1</t>
   </si>
   <si>
     <t>Litr1-2</t>
   </si>
   <si>
-    <t>Phys1-3</t>
+    <t>Litr1-3</t>
   </si>
   <si>
     <t>Math1-4</t>
   </si>
   <si>
-    <t>Litr1-5</t>
-  </si>
-  <si>
-    <t>Math1-1</t>
-  </si>
-  <si>
-    <t>Math1-2</t>
-  </si>
-  <si>
-    <t>Litr1-3</t>
-  </si>
-  <si>
-    <t>Litr1-4</t>
-  </si>
-  <si>
     <t>Math1-5</t>
   </si>
   <si>
+    <t>English2-1</t>
+  </si>
+  <si>
+    <t>Math2-2</t>
+  </si>
+  <si>
+    <t>Phys2-3</t>
+  </si>
+  <si>
+    <t>Phys2-4</t>
+  </si>
+  <si>
+    <t>Phys2-5</t>
+  </si>
+  <si>
     <t>Math2-1</t>
   </si>
   <si>
     <t>Phys2-2</t>
   </si>
   <si>
-    <t>Phys2-3</t>
-  </si>
-  <si>
-    <t>Phys2-4</t>
-  </si>
-  <si>
-    <t>Phys2-5</t>
-  </si>
-  <si>
-    <t>English2-1</t>
-  </si>
-  <si>
-    <t>Math2-2</t>
-  </si>
-  <si>
     <t>Math2-3</t>
   </si>
   <si>
@@ -74,63 +74,63 @@
     <t>Math2-5</t>
   </si>
   <si>
+    <t>Russian3-1</t>
+  </si>
+  <si>
+    <t>Phys3-2</t>
+  </si>
+  <si>
+    <t>English3-3</t>
+  </si>
+  <si>
+    <t>Litra3-4</t>
+  </si>
+  <si>
+    <t>Phys3-5</t>
+  </si>
+  <si>
     <t>English3-1</t>
   </si>
   <si>
-    <t>Phys3-2</t>
-  </si>
-  <si>
-    <t>Russian3-3</t>
+    <t>Russian3-2</t>
+  </si>
+  <si>
+    <t>Phys3-3</t>
   </si>
   <si>
     <t>Phys3-4</t>
   </si>
   <si>
-    <t>English3-5</t>
+    <t>Litra3-5</t>
   </si>
   <si>
     <t>Phys3-1</t>
   </si>
   <si>
-    <t>Russian3-2</t>
-  </si>
-  <si>
-    <t>Phys3-3</t>
-  </si>
-  <si>
-    <t>Litra3-4</t>
-  </si>
-  <si>
-    <t>Phys3-5</t>
-  </si>
-  <si>
-    <t>Russian3-1</t>
-  </si>
-  <si>
     <t>English4-1</t>
   </si>
   <si>
     <t>Phys4-2</t>
   </si>
   <si>
+    <t>Phys4-3</t>
+  </si>
+  <si>
+    <t>Math4-4</t>
+  </si>
+  <si>
+    <t>Math4-5</t>
+  </si>
+  <si>
+    <t>Math4-1</t>
+  </si>
+  <si>
+    <t>English4-2</t>
+  </si>
+  <si>
     <t>Math4-3</t>
   </si>
   <si>
-    <t>Math4-4</t>
-  </si>
-  <si>
-    <t>Math4-5</t>
-  </si>
-  <si>
-    <t>Math4-1</t>
-  </si>
-  <si>
-    <t>Math4-2</t>
-  </si>
-  <si>
-    <t>Phys4-3</t>
-  </si>
-  <si>
     <t>Phys4-4</t>
   </si>
   <si>
@@ -140,13 +140,13 @@
     <t>Russian5-1</t>
   </si>
   <si>
-    <t>Russian5-2</t>
+    <t>Phys5-2</t>
   </si>
   <si>
     <t>Phys5-3</t>
   </si>
   <si>
-    <t>Phys5-4</t>
+    <t>Math5-4</t>
   </si>
   <si>
     <t>Math5-5</t>

</xml_diff>

<commit_message>
TODO init_new + all TODOs
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/test.xlsx
+++ b/src/main/resources/xlsx/test.xlsx
@@ -14,43 +14,58 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
+    <t>Phys1-1</t>
+  </si>
+  <si>
+    <t>Math1-2</t>
+  </si>
+  <si>
+    <t>Phys1-3</t>
+  </si>
+  <si>
+    <t>Litr1-4</t>
+  </si>
+  <si>
+    <t>Math1-5</t>
+  </si>
+  <si>
     <t>Math1-1</t>
   </si>
   <si>
-    <t>Math1-2</t>
-  </si>
-  <si>
-    <t>Phys1-3</t>
-  </si>
-  <si>
-    <t>Litr1-4</t>
+    <t>Litr1-2</t>
+  </si>
+  <si>
+    <t>Litr1-3</t>
+  </si>
+  <si>
+    <t>Math1-4</t>
   </si>
   <si>
     <t>Litr1-5</t>
   </si>
   <si>
-    <t>Phys1-1</t>
-  </si>
-  <si>
-    <t>Litr1-2</t>
-  </si>
-  <si>
-    <t>Litr1-3</t>
-  </si>
-  <si>
-    <t>Math1-4</t>
-  </si>
-  <si>
-    <t>Math1-5</t>
+    <t>Math2-1</t>
+  </si>
+  <si>
+    <t>English2-2</t>
+  </si>
+  <si>
+    <t>Phys2-3</t>
+  </si>
+  <si>
+    <t>English2-4</t>
+  </si>
+  <si>
+    <t>Math2-5</t>
   </si>
   <si>
     <t>English2-1</t>
   </si>
   <si>
-    <t>Math2-2</t>
-  </si>
-  <si>
-    <t>Phys2-3</t>
+    <t>Phys2-2</t>
+  </si>
+  <si>
+    <t>Math2-3</t>
   </si>
   <si>
     <t>Phys2-4</t>
@@ -59,78 +74,63 @@
     <t>Phys2-5</t>
   </si>
   <si>
-    <t>Math2-1</t>
-  </si>
-  <si>
-    <t>Phys2-2</t>
-  </si>
-  <si>
-    <t>Math2-3</t>
-  </si>
-  <si>
-    <t>Math2-4</t>
-  </si>
-  <si>
-    <t>Math2-5</t>
+    <t>Phys3-1</t>
+  </si>
+  <si>
+    <t>Phys3-2</t>
+  </si>
+  <si>
+    <t>Russian3-3</t>
+  </si>
+  <si>
+    <t>Phys3-4</t>
+  </si>
+  <si>
+    <t>English3-5</t>
   </si>
   <si>
     <t>Russian3-1</t>
   </si>
   <si>
-    <t>Phys3-2</t>
-  </si>
-  <si>
-    <t>English3-3</t>
+    <t>Russian3-2</t>
+  </si>
+  <si>
+    <t>Phys3-3</t>
   </si>
   <si>
     <t>Litra3-4</t>
   </si>
   <si>
-    <t>Phys3-5</t>
+    <t>Litra3-5</t>
   </si>
   <si>
     <t>English3-1</t>
   </si>
   <si>
-    <t>Russian3-2</t>
-  </si>
-  <si>
-    <t>Phys3-3</t>
-  </si>
-  <si>
-    <t>Phys3-4</t>
-  </si>
-  <si>
-    <t>Litra3-5</t>
-  </si>
-  <si>
-    <t>Phys3-1</t>
+    <t>Math4-1</t>
+  </si>
+  <si>
+    <t>Phys4-2</t>
+  </si>
+  <si>
+    <t>Math4-3</t>
+  </si>
+  <si>
+    <t>Math4-4</t>
+  </si>
+  <si>
+    <t>Math4-5</t>
   </si>
   <si>
     <t>English4-1</t>
   </si>
   <si>
-    <t>Phys4-2</t>
+    <t>Math4-2</t>
   </si>
   <si>
     <t>Phys4-3</t>
   </si>
   <si>
-    <t>Math4-4</t>
-  </si>
-  <si>
-    <t>Math4-5</t>
-  </si>
-  <si>
-    <t>Math4-1</t>
-  </si>
-  <si>
-    <t>English4-2</t>
-  </si>
-  <si>
-    <t>Math4-3</t>
-  </si>
-  <si>
     <t>Phys4-4</t>
   </si>
   <si>
@@ -146,10 +146,10 @@
     <t>Phys5-3</t>
   </si>
   <si>
-    <t>Math5-4</t>
-  </si>
-  <si>
-    <t>Math5-5</t>
+    <t>Phys5-4</t>
+  </si>
+  <si>
+    <t>Phys5-5</t>
   </si>
 </sst>
 </file>

</xml_diff>